<commit_message>
Updated Ethan's Progress Report
</commit_message>
<xml_diff>
--- a/Progress Reports/EthanRaymond_ProgressReport.xlsx
+++ b/Progress Reports/EthanRaymond_ProgressReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="27315" windowHeight="14820"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,36 @@
   </si>
   <si>
     <t>Editing &amp; Contributing to Report</t>
+  </si>
+  <si>
+    <t>Finishing Code</t>
+  </si>
+  <si>
+    <t>Reviewing Other Group Member's Code</t>
+  </si>
+  <si>
+    <t>Writing Database Interface Functions</t>
+  </si>
+  <si>
+    <t>Create Abstract Page Class</t>
+  </si>
+  <si>
+    <t>Writing Database Interface Functions &amp; Writing JSP Pages</t>
+  </si>
+  <si>
+    <t>Wrote SQL Script for resetting Database</t>
+  </si>
+  <si>
+    <t>Compiled existing SQL scripts into one file</t>
+  </si>
+  <si>
+    <t>Searched for HTML library for java</t>
+  </si>
+  <si>
+    <t>Writing Database Interface Functions &amp; Organized SQL Scripts</t>
+  </si>
+  <si>
+    <t>Created classes to represent database objects</t>
   </si>
 </sst>
 </file>
@@ -578,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,59 +744,125 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
+      <c r="A12" s="15">
+        <v>42825</v>
+      </c>
+      <c r="B12" s="6">
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="A13" s="15">
+        <v>42816</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
+      <c r="A14" s="15">
+        <v>42817</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="15">
+        <v>42832</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="15">
+        <v>42834</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="15">
+        <v>42836</v>
+      </c>
+      <c r="B17" s="6">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="15">
+        <v>42841</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="15">
+        <v>42842</v>
+      </c>
+      <c r="B19" s="6">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="15">
+        <v>42843</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="15">
+        <v>42848</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="12">
+        <v>42852</v>
+      </c>
+      <c r="B22" s="6">
+        <v>14</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -809,9 +905,59 @@
       <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>